<commit_message>
Worked a lot on file, removed old controller, game technically functional, all menus work. Did some light menu designing. Next I really need to clean some controllers and fix some views. First I want to finish the game though, incorporate inventory.
</commit_message>
<xml_diff>
--- a/data/maze_room_themes.xlsx
+++ b/data/maze_room_themes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\denzel\code\DenzelBraithwaite\classy_potion_maker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E30F2E3-C5BF-4F3C-96D0-67C4F5B193E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8CB0CD-0BF8-4B7D-84CE-6BF07BC7E3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6AA14B88-5E0D-4416-822C-0917319A619B}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{6AA14B88-5E0D-4416-822C-0917319A619B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,8 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,187 +454,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DE79B6-A999-49D7-B10C-488C1169C836}">
-  <dimension ref="D3:E25"/>
+  <dimension ref="D3:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" customWidth="1"/>
     <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
+    <row r="3" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D3" s="1"/>
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D5">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D7">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D8">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D9">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D10">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D11">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D20">
-        <v>5</v>
-      </c>
-      <c r="E20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D21">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D22">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D23">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D24">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D25">
-        <v>10</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="G13" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>